<commit_message>
fix: handling error ketika import data fasilitas
</commit_message>
<xml_diff>
--- a/public/template_fasilitas.xlsx
+++ b/public/template_fasilitas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PBL_Fastcili-TI\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2A6DC7-7AB5-4CF9-94A2-6539D171F96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE240F29-B5CE-472B-B209-62E76D73E9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7995" xr2:uid="{627A3C99-4863-4719-B148-124E320C6432}"/>
   </bookViews>
@@ -36,16 +36,16 @@
     <t>jumlah</t>
   </si>
   <si>
-    <t>AC Panasonic NEW</t>
-  </si>
-  <si>
-    <t>Proyektor Epson NEW</t>
-  </si>
-  <si>
-    <t>Kursi NEW</t>
-  </si>
-  <si>
-    <t>Meja NEW</t>
+    <t xml:space="preserve">Proyektor Epson </t>
+  </si>
+  <si>
+    <t>Kursi</t>
+  </si>
+  <si>
+    <t>Meja</t>
+  </si>
+  <si>
+    <t>AC Panasonic</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -478,7 +478,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>8</v>

</xml_diff>

<commit_message>
refactor: merapikan kode impor file
</commit_message>
<xml_diff>
--- a/public/template_fasilitas.xlsx
+++ b/public/template_fasilitas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PBL_Fastcili-TI\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE240F29-B5CE-472B-B209-62E76D73E9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D668FA0-8F46-4735-A04F-2C4471F2F767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7995" xr2:uid="{627A3C99-4863-4719-B148-124E320C6432}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="15375" windowHeight="7995" xr2:uid="{627A3C99-4863-4719-B148-124E320C6432}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +464,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>

</xml_diff>